<commit_message>
Saved file after regenerating schematic from GUI
</commit_message>
<xml_diff>
--- a/Grids_and_profiles/grids/test_temp_correction.xlsx
+++ b/Grids_and_profiles/grids/test_temp_correction.xlsx
@@ -113,10 +113,10 @@
     <t>0.0</t>
   </si>
   <si>
-    <t>-49.33333333333334</t>
-  </si>
-  <si>
-    <t>-73.33333333333333</t>
+    <t>-19.908076343375843</t>
+  </si>
+  <si>
+    <t>-57.80509971944206</t>
   </si>
   <si>
     <t>Defualt</t>
@@ -131,10 +131,10 @@
     <t>False</t>
   </si>
   <si>
-    <t>-40.66666666666666</t>
-  </si>
-  <si>
-    <t>118.66666666666669</t>
+    <t>19.908076343375843</t>
+  </si>
+  <si>
+    <t>57.80509971944206</t>
   </si>
   <si>
     <t>bus_from</t>

</xml_diff>

<commit_message>
Adjusted tooltips; corrected get_save_data()
</commit_message>
<xml_diff>
--- a/Grids_and_profiles/grids/test_temp_correction.xlsx
+++ b/Grids_and_profiles/grids/test_temp_correction.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="116">
   <si>
     <t>Property</t>
   </si>
@@ -212,6 +212,9 @@
     <t>20.0</t>
   </si>
   <si>
+    <t>90.0</t>
+  </si>
+  <si>
     <t>0.00323</t>
   </si>
   <si>
@@ -242,9 +245,6 @@
     <t>Load0</t>
   </si>
   <si>
-    <t>0.4</t>
-  </si>
-  <si>
     <t>is_controlled</t>
   </si>
   <si>
@@ -297,15 +297,6 @@
   </si>
   <si>
     <t>utility</t>
-  </si>
-  <si>
-    <t>0.8</t>
-  </si>
-  <si>
-    <t>9999.0</t>
-  </si>
-  <si>
-    <t>-9999.0</t>
   </si>
   <si>
     <t>wire_name</t>
@@ -813,58 +804,58 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="B1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -903,16 +894,16 @@
         <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -951,16 +942,16 @@
         <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -987,25 +978,25 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1323,10 +1314,10 @@
         <v>60</v>
       </c>
       <c r="S2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="T2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U2" t="s">
         <v>27</v>
@@ -1335,13 +1326,13 @@
         <v>27</v>
       </c>
       <c r="W2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="X2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="Y2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1368,22 +1359,22 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>43</v>
@@ -1403,37 +1394,37 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1447,7 +1438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:F1"/>
+  <dimension ref="B1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1455,20 +1446,26 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1496,7 +1493,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -1505,7 +1502,7 @@
         <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>73</v>
@@ -1586,7 +1583,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -1595,7 +1592,7 @@
         <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>73</v>
@@ -1641,47 +1638,47 @@
       <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K2" t="s">
-        <v>91</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" t="s">
-        <v>91</v>
-      </c>
-      <c r="N2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>27</v>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>9999</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-9999</v>
+      </c>
+      <c r="K2" t="n">
+        <v>9999</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>9999</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1708,7 +1705,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -1747,25 +1744,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>